<commit_message>
Add all 128 size trained model weights
</commit_message>
<xml_diff>
--- a/performance.xlsx
+++ b/performance.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jumpr_000\Desktop\alignment-lstm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\alignment-classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="16">
   <si>
     <t>h3</t>
   </si>
@@ -50,16 +50,25 @@
     <t>h3k79me3</t>
   </si>
   <si>
-    <t>jaist</t>
-  </si>
-  <si>
     <t>h4</t>
   </si>
   <si>
     <t>h4ac</t>
   </si>
   <si>
-    <t>10 epochs:</t>
+    <t>15 epochs, 128 kernels:</t>
+  </si>
+  <si>
+    <t>Best:</t>
+  </si>
+  <si>
+    <t>this paper</t>
+  </si>
+  <si>
+    <t>Pham et al.</t>
+  </si>
+  <si>
+    <t>Ngoc Giang et al.</t>
   </si>
   <si>
     <t>15 epochs:</t>
@@ -142,6 +151,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>128:256 Convolution Kernels</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -184,7 +218,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>Sheet1!$B$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -205,7 +239,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Sheet1!$A$17:$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -243,46 +277,46 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:f>Sheet1!$B$17:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>81.2</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>66.099999999999994</c:v>
+                  <c:v>70.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68.599999999999994</c:v>
+                  <c:v>71.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.2</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>58.9</c:v>
+                  <c:v>73.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>66.5</c:v>
+                  <c:v>57.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>71.099999999999994</c:v>
+                  <c:v>70.7</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>70.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>86.1</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>65.3</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FA12-400D-ACE6-8238BA07DFDD}"/>
+              <c16:uniqueId val="{00000000-B15C-414A-852B-7BD401EEAB1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -291,7 +325,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Sheet1!$C$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -312,7 +346,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Sheet1!$A$17:$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -350,46 +384,46 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$12</c:f>
+              <c:f>Sheet1!$C$17:$C$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>82.1</c:v>
+                  <c:v>87.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.9</c:v>
+                  <c:v>72.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.3</c:v>
+                  <c:v>64.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>59.6</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63</c:v>
+                  <c:v>68.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>70.2</c:v>
+                  <c:v>73.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>57.8</c:v>
+                  <c:v>68.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>75.900000000000006</c:v>
+                  <c:v>78.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>62</c:v>
+                  <c:v>90.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>62.2</c:v>
+                  <c:v>75.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FA12-400D-ACE6-8238BA07DFDD}"/>
+              <c16:uniqueId val="{00000001-B15C-414A-852B-7BD401EEAB1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -398,7 +432,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>Sheet1!$D$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -419,7 +453,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Sheet1!$A$17:$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -457,46 +491,46 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$12</c:f>
+              <c:f>Sheet1!$D$17:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>78.400000000000006</c:v>
+                  <c:v>86.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>59.6</c:v>
+                  <c:v>74.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.599999999999994</c:v>
+                  <c:v>69.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>53</c:v>
+                  <c:v>54.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63.5</c:v>
+                  <c:v>78.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.8</c:v>
+                  <c:v>78.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72.8</c:v>
+                  <c:v>78.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>56.5</c:v>
+                  <c:v>73.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>90.1</c:v>
+                  <c:v>92.7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>67.5</c:v>
+                  <c:v>76.400000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FA12-400D-ACE6-8238BA07DFDD}"/>
+              <c16:uniqueId val="{00000002-B15C-414A-852B-7BD401EEAB1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -505,7 +539,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Sheet1!$E$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -526,7 +560,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Sheet1!$A$17:$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -564,46 +598,46 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$12</c:f>
+              <c:f>Sheet1!$E$17:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>88.9</c:v>
+                  <c:v>90.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>63.6</c:v>
+                  <c:v>74.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.8</c:v>
+                  <c:v>70.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64</c:v>
+                  <c:v>50.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.400000000000006</c:v>
+                  <c:v>84.7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>58</c:v>
+                  <c:v>66.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>65.099999999999994</c:v>
+                  <c:v>82.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57.8</c:v>
+                  <c:v>80.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>69.400000000000006</c:v>
+                  <c:v>73.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>68.2</c:v>
+                  <c:v>70.599999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-FA12-400D-ACE6-8238BA07DFDD}"/>
+              <c16:uniqueId val="{00000003-B15C-414A-852B-7BD401EEAB1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -612,11 +646,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$2</c:f>
+              <c:f>Sheet1!$F$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>jaist</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -633,7 +667,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:f>Sheet1!$A$17:$A$26</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -671,46 +705,46 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$12</c:f>
+              <c:f>Sheet1!$F$17:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>86.4</c:v>
+                  <c:v>92.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72.400000000000006</c:v>
+                  <c:v>82.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.3</c:v>
+                  <c:v>79.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.5</c:v>
+                  <c:v>75.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>77.5</c:v>
+                  <c:v>66.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>76.3</c:v>
+                  <c:v>80.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>77.099999999999994</c:v>
+                  <c:v>73.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>82.6</c:v>
+                  <c:v>79.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>88.1</c:v>
+                  <c:v>94.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>75.599999999999994</c:v>
+                  <c:v>82.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-FA12-400D-ACE6-8238BA07DFDD}"/>
+              <c16:uniqueId val="{00000004-B15C-414A-852B-7BD401EEAB1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -724,11 +758,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="617661600"/>
-        <c:axId val="617660288"/>
+        <c:axId val="482473512"/>
+        <c:axId val="482479088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="617661600"/>
+        <c:axId val="482473512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -771,7 +805,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="617660288"/>
+        <c:crossAx val="482479088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -779,9 +813,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="617660288"/>
+        <c:axId val="482479088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="50"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -830,7 +865,609 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="617661600"/>
+        <c:crossAx val="482473512"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Compared to Previous Work</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>this paper</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$31:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>h3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>h3k4me1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>h3k4me2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>h3k4me3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>h3k9ac</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>h3k14ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>h3k36me3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>h3k79me3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>h4ac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$31:$B$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>92.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>82.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>84.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>94.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BE3A-41D8-A4B3-8C73E9A8E4C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ngoc Giang et al.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$31:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>h3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>h3k4me1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>h3k4me2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>h3k4me3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>h3k9ac</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>h3k14ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>h3k36me3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>h3k79me3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>h4ac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$31:$C$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>89.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>74.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83.3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>77.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BE3A-41D8-A4B3-8C73E9A8E4C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pham et al.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$31:$A$40</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>h3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>h3k4me1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>h3k4me2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>h3k4me3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>h3k9ac</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>h3k14ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>h3k36me3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>h3k79me3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>h4ac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$31:$D$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>86.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>82.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>75.599999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BE3A-41D8-A4B3-8C73E9A8E4C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="483983232"/>
+        <c:axId val="483982904"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="483983232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="483982904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="483982904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="483983232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -911,7 +1548,898 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>64:128 Convolution Kernels</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>h3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>h3k4me1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>h3k4me2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>h3k4me3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>h3k9ac</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>h3k14ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>h3k36me3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>h3k79me3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>h4ac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$3:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>85.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>61.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70.900000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D1C0-47D5-83E0-F350C493D289}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>h3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>h3k4me1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>h3k4me2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>h3k4me3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>h3k9ac</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>h3k14ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>h3k36me3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>h3k79me3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>h4ac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>85.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>74.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>86.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D1C0-47D5-83E0-F350C493D289}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>h3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>h3k4me1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>h3k4me2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>h3k4me3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>h3k9ac</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>h3k14ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>h3k36me3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>h3k79me3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>h4ac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$3:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>77.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>61.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>85.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>72.400000000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D1C0-47D5-83E0-F350C493D289}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>h3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>h3k4me1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>h3k4me2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>h3k4me3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>h3k9ac</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>h3k14ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>h3k36me3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>h3k79me3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>h4ac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$3:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>83.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>78.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>71.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D1C0-47D5-83E0-F350C493D289}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$3:$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>h3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>h3k4me1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>h3k4me2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>h3k4me3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>h3k9ac</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>h3k14ac</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>h3k36me3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>h3k79me3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>h4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>h4ac</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>90.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.599999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>76.099999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D1C0-47D5-83E0-F350C493D289}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="374853400"/>
+        <c:axId val="374850120"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="374853400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="374850120"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="374850120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="374853400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1454,24 +2982,1030 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>276226</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1486,7 +4020,211 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.22278</cdr:x>
+      <cdr:y>0.89757</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.46278</cdr:x>
+      <cdr:y>0.98611</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1018540" y="2626360"/>
+          <a:ext cx="1097280" cy="259080"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="900"/>
+            <a:t>kernel size:</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.2284</cdr:x>
+      <cdr:y>0.88475</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.49857</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1045984" y="2373100"/>
+          <a:ext cx="1237271" cy="309140"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="900"/>
+            <a:t>kernel size:</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1752,20 +4490,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>4</v>
       </c>
@@ -1778,31 +4516,31 @@
       <c r="E2">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
+      <c r="F2">
+        <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>81.2</v>
+        <v>85.9</v>
       </c>
       <c r="C3">
-        <v>82.1</v>
+        <v>85.1</v>
       </c>
       <c r="D3">
-        <v>78.400000000000006</v>
-      </c>
-      <c r="E3" s="1">
-        <v>88.9</v>
-      </c>
-      <c r="F3">
-        <v>86.4</v>
+        <v>77.900000000000006</v>
+      </c>
+      <c r="E3" s="2">
+        <v>83.8</v>
+      </c>
+      <c r="F3" s="1">
+        <v>90.8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1810,323 +4548,571 @@
         <v>66.099999999999994</v>
       </c>
       <c r="C4">
-        <v>63.9</v>
+        <v>52.7</v>
       </c>
       <c r="D4">
-        <v>59.6</v>
-      </c>
-      <c r="E4">
-        <v>63.6</v>
+        <v>68</v>
+      </c>
+      <c r="E4" s="2">
+        <v>70.900000000000006</v>
       </c>
       <c r="F4" s="1">
-        <v>72.400000000000006</v>
-      </c>
+        <v>76.599999999999994</v>
+      </c>
+      <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
-        <v>68.599999999999994</v>
+        <v>61.8</v>
       </c>
       <c r="C5">
-        <v>69.3</v>
+        <v>57.1</v>
       </c>
       <c r="D5">
-        <v>69.599999999999994</v>
-      </c>
-      <c r="E5">
-        <v>70.8</v>
-      </c>
-      <c r="F5" s="1">
-        <v>71.3</v>
-      </c>
+        <v>71.5</v>
+      </c>
+      <c r="E5" s="1">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="F5" s="2">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
-        <v>60.2</v>
+        <v>63.8</v>
       </c>
       <c r="C6">
-        <v>59.6</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="D6">
-        <v>53</v>
-      </c>
-      <c r="E6">
-        <v>64</v>
-      </c>
-      <c r="F6" s="1">
-        <v>72.5</v>
-      </c>
+        <v>66.8</v>
+      </c>
+      <c r="E6" s="2">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="F6" s="2">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>58.9</v>
+        <v>75.400000000000006</v>
       </c>
       <c r="C7">
-        <v>63</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="D7">
-        <v>63.5</v>
-      </c>
-      <c r="E7">
-        <v>76.400000000000006</v>
+        <v>77.900000000000006</v>
+      </c>
+      <c r="E7" s="2">
+        <v>78.599999999999994</v>
       </c>
       <c r="F7" s="1">
-        <v>77.5</v>
-      </c>
+        <v>81.8</v>
+      </c>
+      <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8">
-        <v>66.5</v>
+        <v>67.5</v>
       </c>
       <c r="C8">
-        <v>70.2</v>
+        <v>72</v>
       </c>
       <c r="D8">
-        <v>62.8</v>
-      </c>
-      <c r="E8">
-        <v>58</v>
+        <v>71.900000000000006</v>
+      </c>
+      <c r="E8" s="2">
+        <v>60.8</v>
       </c>
       <c r="F8" s="1">
-        <v>76.3</v>
-      </c>
+        <v>77.2</v>
+      </c>
+      <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
-        <v>71.099999999999994</v>
+        <v>65</v>
       </c>
       <c r="C9">
-        <v>57.8</v>
+        <v>73.400000000000006</v>
       </c>
       <c r="D9">
-        <v>72.8</v>
-      </c>
-      <c r="E9">
-        <v>65.099999999999994</v>
+        <v>75.400000000000006</v>
+      </c>
+      <c r="E9" s="2">
+        <v>71.7</v>
       </c>
       <c r="F9" s="1">
-        <v>77.099999999999994</v>
-      </c>
+        <v>79.900000000000006</v>
+      </c>
+      <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="C10">
+        <v>74.7</v>
+      </c>
+      <c r="D10">
+        <v>61.6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="F10" s="1">
+        <v>85.4</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>72.8</v>
+      </c>
+      <c r="C11">
+        <v>86.4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>85.2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>90.2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>90.7</v>
+      </c>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="C12">
+        <v>60.6</v>
+      </c>
+      <c r="D12" s="2">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="E12" s="2">
+        <v>71.3</v>
+      </c>
+      <c r="F12" s="1">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>16</v>
+      </c>
+      <c r="F16">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>90</v>
+      </c>
+      <c r="C17">
+        <v>87.1</v>
+      </c>
+      <c r="D17">
+        <v>86.1</v>
+      </c>
+      <c r="E17" s="2">
+        <v>90.4</v>
+      </c>
+      <c r="F17" s="1">
+        <v>92.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>70.2</v>
+      </c>
+      <c r="C18">
+        <v>72.5</v>
+      </c>
+      <c r="D18">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="E18" s="2">
+        <v>74.5</v>
+      </c>
+      <c r="F18" s="1">
+        <v>82.1</v>
+      </c>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>71.3</v>
+      </c>
+      <c r="C19">
+        <v>64.2</v>
+      </c>
+      <c r="D19">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="E19" s="2">
+        <v>70.5</v>
+      </c>
+      <c r="F19" s="1">
+        <v>79.5</v>
+      </c>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>64</v>
+      </c>
+      <c r="C20">
+        <v>54</v>
+      </c>
+      <c r="D20">
+        <v>54.4</v>
+      </c>
+      <c r="E20" s="2">
+        <v>50.1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>75.3</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>73.3</v>
+      </c>
+      <c r="C21">
+        <v>68.3</v>
+      </c>
+      <c r="D21">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="E21" s="1">
+        <v>84.7</v>
+      </c>
+      <c r="F21" s="2">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>57.9</v>
+      </c>
+      <c r="C22">
+        <v>73.8</v>
+      </c>
+      <c r="D22">
+        <v>78.2</v>
+      </c>
+      <c r="E22" s="2">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="F22" s="1">
+        <v>80.8</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>70.7</v>
+      </c>
+      <c r="C23">
+        <v>68.5</v>
+      </c>
+      <c r="D23">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="E23" s="1">
+        <v>82.4</v>
+      </c>
+      <c r="F23" s="2">
+        <v>73.5</v>
+      </c>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
         <v>70.599999999999994</v>
       </c>
-      <c r="C10">
-        <v>75.900000000000006</v>
-      </c>
-      <c r="D10">
-        <v>56.5</v>
-      </c>
-      <c r="E10">
-        <v>57.8</v>
-      </c>
-      <c r="F10" s="1">
+      <c r="C24">
+        <v>78.8</v>
+      </c>
+      <c r="D24">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="E24">
+        <v>80.3</v>
+      </c>
+      <c r="F24" s="2">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
+        <v>82</v>
+      </c>
+      <c r="C25">
+        <v>90.3</v>
+      </c>
+      <c r="D25" s="2">
+        <v>92.7</v>
+      </c>
+      <c r="E25">
+        <v>73.8</v>
+      </c>
+      <c r="F25" s="1">
+        <v>94.9</v>
+      </c>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26">
+        <v>74</v>
+      </c>
+      <c r="C26">
+        <v>75.7</v>
+      </c>
+      <c r="D26">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="E26">
+        <v>70.599999999999994</v>
+      </c>
+      <c r="F26" s="1">
+        <v>82.2</v>
+      </c>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>92.7</v>
+      </c>
+      <c r="C31">
+        <v>89.2</v>
+      </c>
+      <c r="D31">
+        <v>86.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>82.1</v>
+      </c>
+      <c r="C32">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="D32" s="2">
+        <v>72.400000000000006</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33">
+        <v>79.5</v>
+      </c>
+      <c r="C33">
+        <v>71.8</v>
+      </c>
+      <c r="D33" s="2">
+        <v>71.3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>75.3</v>
+      </c>
+      <c r="C34">
+        <v>74.8</v>
+      </c>
+      <c r="D34" s="2">
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>84.7</v>
+      </c>
+      <c r="C35">
+        <v>79.290000000000006</v>
+      </c>
+      <c r="D35" s="2">
+        <v>77.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>80.8</v>
+      </c>
+      <c r="C36">
+        <v>78.3</v>
+      </c>
+      <c r="D36" s="2">
+        <v>76.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>82.4</v>
+      </c>
+      <c r="C37">
+        <v>79.3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>77.099999999999994</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>85.4</v>
+      </c>
+      <c r="C38">
+        <v>83.3</v>
+      </c>
+      <c r="D38" s="2">
         <v>82.6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39">
+        <v>94.9</v>
+      </c>
+      <c r="C39">
+        <v>88.3</v>
+      </c>
+      <c r="D39" s="2">
+        <v>88.1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>86.1</v>
-      </c>
-      <c r="C11">
-        <v>62</v>
-      </c>
-      <c r="D11" s="1">
-        <v>90.1</v>
-      </c>
-      <c r="E11">
-        <v>69.400000000000006</v>
-      </c>
-      <c r="F11" s="2">
-        <v>88.1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>65.3</v>
-      </c>
-      <c r="C12">
-        <v>62.2</v>
-      </c>
-      <c r="D12">
-        <v>67.5</v>
-      </c>
-      <c r="E12">
-        <v>68.2</v>
-      </c>
-      <c r="F12" s="1">
-        <v>75.599999999999994</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>10</v>
-      </c>
-      <c r="E15">
-        <v>16</v>
-      </c>
-      <c r="F15">
-        <v>32</v>
-      </c>
-      <c r="G15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>85.9</v>
-      </c>
-      <c r="C16">
-        <v>85.1</v>
-      </c>
-      <c r="D16">
-        <v>77.900000000000006</v>
-      </c>
-      <c r="E16" s="2">
-        <v>83.8</v>
-      </c>
-      <c r="F16" s="1">
-        <v>90.8</v>
-      </c>
-      <c r="G16">
-        <v>86.4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17">
-        <v>66.099999999999994</v>
-      </c>
-      <c r="C17">
-        <v>52.7</v>
-      </c>
-      <c r="D17">
-        <v>68</v>
-      </c>
-      <c r="E17" s="2">
-        <v>70.900000000000006</v>
-      </c>
-      <c r="F17" s="1">
-        <v>76.599999999999994</v>
-      </c>
-      <c r="G17" s="2">
-        <v>72.400000000000006</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18">
-        <v>61.8</v>
-      </c>
-      <c r="C18">
-        <v>57.1</v>
-      </c>
-      <c r="D18">
-        <v>71.5</v>
-      </c>
-      <c r="E18" s="2">
-        <v>72.900000000000006</v>
-      </c>
-      <c r="G18" s="2">
-        <v>71.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="1">
-        <v>72.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="1">
+      <c r="B40">
+        <v>82.2</v>
+      </c>
+      <c r="C40">
         <v>77.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-      <c r="G21" s="1">
-        <v>76.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="1">
-        <v>77.099999999999994</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>7</v>
-      </c>
-      <c r="G23" s="1">
-        <v>82.6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="G24" s="2">
-        <v>88.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G25" s="1">
+      <c r="D40" s="2">
         <v>75.599999999999994</v>
       </c>
     </row>

</xml_diff>